<commit_message>
Tela do servidor pronta
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_entrada_itens.xlsx
+++ b/relatorios/relatorio_entrada_itens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="27" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,19 +469,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sabão em barra</t>
+          <t>Sabão Líquido</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>29/05/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -492,122 +492,122 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cabo USB</t>
+          <t>Borracha Branca</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>29/05/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Informática</t>
+          <t>Limpeza</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lápis</t>
+          <t>Chave de fenda</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>29/05/2025</t>
+          <t>02/06/2025</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Papelaria</t>
+          <t>FERRAMENTAS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Apagador</t>
+          <t>Caderno Espiral</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>29/05/2025</t>
+          <t>02/06/2025</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Materiais Sala de Aula</t>
+          <t>Papelaria</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TESTE</t>
+          <t>Borracha Branca</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15/05/2025</t>
+          <t>02/06/2025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Informática</t>
+          <t>Papelaria</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chave de fenda</t>
+          <t>Papel A1 Sulfite</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>02/06/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>FERRAMENTAS</t>
+          <t>Limpeza</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -615,26 +615,26 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>299</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>02/06/2025</t>
+          <t>03/06/2025</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Papelaria</t>
+          <t>Limpeza</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Borracha Branca</t>
+          <t>Garrafa de Água</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -642,49 +642,49 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>02/06/2025</t>
+          <t>04/06/2025</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Papelaria</t>
+          <t>Diversos</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Detergente</t>
+          <t>Caneta Esferográfica Azul</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>300</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>28/05/2025</t>
+          <t>02/06/2025</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Limpeza</t>
+          <t>Papelaria</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sabão Líquido</t>
+          <t>Caderno Espiral</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -693,21 +693,21 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Limpeza</t>
+          <t>Material Escolar</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Caderno Espiral</t>
+          <t>Papel A4 Sulfite</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -716,306 +716,30 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Limpeza</t>
+          <t>Papelaria</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Papel A1 Sulfite</t>
+          <t>Açúcar</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>02/06/2025</t>
+          <t>04/06/2025</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Limpeza</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>92</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Borracha Branca</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>40</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>02/06/2025</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Limpeza</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>83</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Caneta Esferográfica Azul</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>300</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>02/06/2025</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>67</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Mouse USB</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>28/05/2025</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Informática</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>87</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Caderno Espiral</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>100</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>02/06/2025</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Material Escolar</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>75</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Cabo VGA</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>27/05/2025</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Informática</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>85</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Papel A4 Sulfite</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>15</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>02/06/2025</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>88</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Borracha Branca</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>40</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>02/06/2025</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Material Escolar</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>63</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Caneta Preta</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>14/05/2025</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>65</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Caneta Azul</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>4</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>14/05/2025</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>76</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Sabão em Pó</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>28/05/2025</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Limpeza</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>68</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Teclado USB</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>14/05/2025</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Informática</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>66</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Caneta Vermelha</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>100</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>14/05/2025</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
+          <t>Diversos</t>
         </is>
       </c>
     </row>

</xml_diff>